<commit_message>
UCUA Latest Print sheet
</commit_message>
<xml_diff>
--- a/RAMS/Web/RAMMS.Web.UI/wwwroot/Templates/FORMUCUA.xlsx
+++ b/RAMS/Web/RAMMS.Web.UI/wwwroot/Templates/FORMUCUA.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Table 1'!$A$1:$P$32</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Table 1'!$A$1:$P$33</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -702,7 +702,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -718,6 +718,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -886,31 +889,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1308,10 +1305,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:P32"/>
+  <dimension ref="B1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A27" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31:O31"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
@@ -1328,590 +1325,605 @@
     <col min="10" max="10" width="1.19921875" customWidth="1"/>
     <col min="11" max="11" width="9.296875" customWidth="1"/>
     <col min="12" max="12" width="14" customWidth="1"/>
-    <col min="13" max="13" width="12.19921875" customWidth="1"/>
+    <col min="13" max="13" width="1.19921875" customWidth="1"/>
     <col min="14" max="14" width="22" customWidth="1"/>
     <col min="15" max="15" width="1.19921875" customWidth="1"/>
     <col min="16" max="16" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:16" ht="95.5" customHeight="1">
-      <c r="B1" s="48"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
-      <c r="P1" s="49"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
+      <c r="P1" s="50"/>
     </row>
     <row r="2" spans="2:16" ht="6.75" customHeight="1">
       <c r="B2" s="1"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="52"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="53"/>
       <c r="P2" s="1"/>
     </row>
     <row r="3" spans="2:16" ht="25.5" customHeight="1">
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="54"/>
-      <c r="O3" s="55"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="56"/>
       <c r="P3" s="3"/>
     </row>
     <row r="4" spans="2:16" ht="15.75" customHeight="1">
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="57"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="24"/>
-      <c r="O4" s="24"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="25"/>
       <c r="P4" s="1"/>
     </row>
     <row r="5" spans="2:16" ht="32.25" customHeight="1">
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="58"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="58"/>
-      <c r="K5" s="58"/>
-      <c r="L5" s="58"/>
-      <c r="M5" s="58"/>
-      <c r="N5" s="58"/>
-      <c r="O5" s="59"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="59"/>
+      <c r="L5" s="59"/>
+      <c r="M5" s="59"/>
+      <c r="N5" s="59"/>
+      <c r="O5" s="60"/>
       <c r="P5" s="3"/>
     </row>
     <row r="6" spans="2:16" ht="15.75" customHeight="1">
-      <c r="B6" s="56"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="24"/>
-      <c r="O6" s="24"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="25"/>
       <c r="P6" s="1"/>
     </row>
     <row r="7" spans="2:16" ht="33" customHeight="1">
-      <c r="B7" s="56"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="58"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="58"/>
-      <c r="J7" s="58"/>
-      <c r="K7" s="58"/>
-      <c r="L7" s="58"/>
-      <c r="M7" s="58"/>
-      <c r="N7" s="58"/>
-      <c r="O7" s="59"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="59"/>
+      <c r="H7" s="59"/>
+      <c r="I7" s="59"/>
+      <c r="J7" s="59"/>
+      <c r="K7" s="59"/>
+      <c r="L7" s="59"/>
+      <c r="M7" s="59"/>
+      <c r="N7" s="59"/>
+      <c r="O7" s="60"/>
       <c r="P7" s="3"/>
     </row>
     <row r="8" spans="2:16" ht="26.15" customHeight="1">
-      <c r="B8" s="56"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
+      <c r="B8" s="57"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
       <c r="I8" s="3"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="34"/>
-      <c r="L8" s="34"/>
-      <c r="M8" s="34"/>
-      <c r="N8" s="34"/>
-      <c r="O8" s="34"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="35"/>
+      <c r="N8" s="35"/>
+      <c r="O8" s="35"/>
       <c r="P8" s="3"/>
     </row>
     <row r="9" spans="2:16" ht="31.5" customHeight="1">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="11"/>
       <c r="P9" s="3"/>
     </row>
     <row r="10" spans="2:16" ht="32.25" customHeight="1">
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="42"/>
-      <c r="L10" s="42"/>
-      <c r="M10" s="42"/>
-      <c r="N10" s="42"/>
-      <c r="O10" s="43"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="43"/>
+      <c r="O10" s="44"/>
       <c r="P10" s="3"/>
     </row>
     <row r="11" spans="2:16" ht="31.5" customHeight="1">
       <c r="B11" s="4"/>
-      <c r="C11" s="41" t="s">
+      <c r="C11" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="44"/>
       <c r="I11" s="4"/>
-      <c r="J11" s="41" t="s">
+      <c r="J11" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="K11" s="42"/>
-      <c r="L11" s="42"/>
-      <c r="M11" s="42"/>
-      <c r="N11" s="42"/>
-      <c r="O11" s="43"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="43"/>
+      <c r="M11" s="43"/>
+      <c r="N11" s="43"/>
+      <c r="O11" s="44"/>
       <c r="P11" s="3"/>
     </row>
     <row r="12" spans="2:16" ht="184" customHeight="1">
-      <c r="B12" s="44"/>
-      <c r="C12" s="45"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="47"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="19"/>
-      <c r="O12" s="20"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="21"/>
       <c r="P12" s="2"/>
     </row>
     <row r="13" spans="2:16" ht="17.5" customHeight="1">
       <c r="B13" s="1"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="24"/>
-      <c r="L13" s="24"/>
-      <c r="M13" s="24"/>
-      <c r="N13" s="24"/>
-      <c r="O13" s="24"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="25"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
+      <c r="O13" s="25"/>
       <c r="P13" s="1"/>
     </row>
     <row r="14" spans="2:16" ht="31.5" customHeight="1">
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="11"/>
       <c r="P14" s="3"/>
     </row>
     <row r="15" spans="2:16" ht="149.9" customHeight="1">
-      <c r="B15" s="21"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="22"/>
-      <c r="L15" s="22"/>
-      <c r="M15" s="22"/>
-      <c r="N15" s="22"/>
-      <c r="O15" s="23"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="24"/>
       <c r="P15" s="2"/>
     </row>
     <row r="16" spans="2:16" ht="90" customHeight="1">
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
       <c r="P16" s="2"/>
     </row>
     <row r="17" spans="2:16" ht="95.25" customHeight="1">
-      <c r="B17" s="40"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
-      <c r="K17" s="40"/>
-      <c r="L17" s="40"/>
-      <c r="M17" s="40"/>
-      <c r="N17" s="40"/>
-      <c r="O17" s="40"/>
-      <c r="P17" s="5"/>
+      <c r="B17" s="41"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="41"/>
+      <c r="K17" s="41"/>
+      <c r="L17" s="41"/>
+      <c r="M17" s="41"/>
+      <c r="N17" s="41"/>
+      <c r="O17" s="41"/>
+      <c r="P17" s="6"/>
     </row>
     <row r="18" spans="2:16" ht="35.5" customHeight="1">
-      <c r="B18" s="35" t="s">
+      <c r="B18" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="36"/>
-      <c r="J18" s="36"/>
-      <c r="K18" s="36"/>
-      <c r="L18" s="36"/>
-      <c r="M18" s="36"/>
-      <c r="N18" s="37"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="37"/>
+      <c r="L18" s="37"/>
+      <c r="M18" s="37"/>
+      <c r="N18" s="38"/>
       <c r="O18" s="3"/>
       <c r="P18" s="3"/>
     </row>
     <row r="19" spans="2:16" ht="42.75" customHeight="1">
-      <c r="B19" s="38" t="s">
+      <c r="B19" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="38"/>
+      <c r="C19" s="39"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="38" t="s">
+      <c r="I19" s="35"/>
+      <c r="J19" s="35"/>
+      <c r="K19" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="L19" s="38"/>
+      <c r="L19" s="39"/>
       <c r="M19" s="3"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
     </row>
     <row r="20" spans="2:16" ht="23.15" customHeight="1">
-      <c r="B20" s="24"/>
-      <c r="C20" s="24"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="39"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="24"/>
-      <c r="J20" s="24"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="25"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
     </row>
     <row r="21" spans="2:16" ht="15" customHeight="1">
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
-      <c r="L21" s="17"/>
-      <c r="M21" s="17"/>
-      <c r="N21" s="17"/>
-      <c r="O21" s="18"/>
-      <c r="P21" s="6"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="7"/>
     </row>
     <row r="22" spans="2:16" ht="58.5" customHeight="1">
-      <c r="B22" s="25"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="26"/>
-      <c r="K22" s="26"/>
-      <c r="L22" s="26"/>
-      <c r="M22" s="26"/>
-      <c r="N22" s="26"/>
-      <c r="O22" s="27"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="27"/>
+      <c r="M22" s="27"/>
+      <c r="N22" s="27"/>
+      <c r="O22" s="28"/>
       <c r="P22" s="2"/>
     </row>
-    <row r="23" spans="2:16" ht="29.5" customHeight="1">
-      <c r="B23" s="28" t="s">
+    <row r="23" spans="2:16" ht="32.25" customHeight="1">
+      <c r="B23" s="29"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="31"/>
+      <c r="L23" s="32"/>
+      <c r="M23" s="33"/>
+      <c r="N23" s="33"/>
+      <c r="O23" s="34"/>
+      <c r="P23" s="5"/>
+    </row>
+    <row r="24" spans="2:16" ht="29.5" customHeight="1">
+      <c r="B24" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="28" t="s">
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="I23" s="29"/>
-      <c r="J23" s="29"/>
-      <c r="K23" s="30"/>
-      <c r="L23" s="31" t="s">
+      <c r="I24" s="30"/>
+      <c r="J24" s="30"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="M23" s="32"/>
-      <c r="N23" s="32"/>
-      <c r="O23" s="33"/>
-      <c r="P23" s="3"/>
-    </row>
-    <row r="24" spans="2:16" ht="27" customHeight="1">
-      <c r="B24" s="65"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="65"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="65"/>
-      <c r="G24" s="65"/>
-      <c r="H24" s="65"/>
-      <c r="I24" s="65"/>
-      <c r="J24" s="65"/>
-      <c r="K24" s="65"/>
-      <c r="L24" s="65"/>
-      <c r="M24" s="65"/>
-      <c r="N24" s="65"/>
-      <c r="O24" s="3"/>
+      <c r="M24" s="33"/>
+      <c r="N24" s="33"/>
+      <c r="O24" s="34"/>
       <c r="P24" s="3"/>
     </row>
-    <row r="25" spans="2:16" ht="31.5" customHeight="1">
-      <c r="B25" s="8" t="s">
+    <row r="25" spans="2:16" ht="27" customHeight="1">
+      <c r="B25" s="35"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="35"/>
+      <c r="J25" s="35"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+    </row>
+    <row r="26" spans="2:16" ht="31.5" customHeight="1">
+      <c r="B26" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
-      <c r="M25" s="9"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="10"/>
-      <c r="P25" s="3"/>
-    </row>
-    <row r="26" spans="2:16" ht="20.149999999999999" customHeight="1">
-      <c r="B26" s="68" t="s">
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="3"/>
+    </row>
+    <row r="27" spans="2:16" ht="20.149999999999999" customHeight="1">
+      <c r="B27" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="69"/>
-      <c r="D26" s="69"/>
-      <c r="E26" s="69"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="43"/>
-      <c r="I26" s="68" t="s">
+      <c r="C27" s="63"/>
+      <c r="D27" s="63"/>
+      <c r="E27" s="63"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="43"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="J26" s="69"/>
-      <c r="K26" s="69"/>
-      <c r="L26" s="42"/>
-      <c r="M26" s="42"/>
-      <c r="N26" s="42"/>
-      <c r="O26" s="60"/>
-      <c r="P26" s="1"/>
-    </row>
-    <row r="27" spans="2:16" ht="99.65" customHeight="1">
-      <c r="B27" s="21"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
-      <c r="K27" s="22"/>
-      <c r="L27" s="22"/>
-      <c r="M27" s="22"/>
-      <c r="N27" s="22"/>
-      <c r="O27" s="23"/>
-      <c r="P27" s="2"/>
-    </row>
-    <row r="28" spans="2:16" ht="17.149999999999999" customHeight="1">
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
-      <c r="N28" s="1"/>
-      <c r="O28" s="1"/>
-      <c r="P28" s="1"/>
-    </row>
-    <row r="29" spans="2:16" ht="31.5" customHeight="1">
-      <c r="B29" s="8" t="s">
+      <c r="J27" s="63"/>
+      <c r="K27" s="63"/>
+      <c r="L27" s="43"/>
+      <c r="M27" s="43"/>
+      <c r="N27" s="43"/>
+      <c r="O27" s="61"/>
+      <c r="P27" s="1"/>
+    </row>
+    <row r="28" spans="2:16" ht="99.65" customHeight="1">
+      <c r="B28" s="22"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="23"/>
+      <c r="L28" s="23"/>
+      <c r="M28" s="23"/>
+      <c r="N28" s="23"/>
+      <c r="O28" s="24"/>
+      <c r="P28" s="2"/>
+    </row>
+    <row r="29" spans="2:16" ht="17.149999999999999" customHeight="1">
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="25"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+    </row>
+    <row r="30" spans="2:16" ht="31.5" customHeight="1">
+      <c r="B30" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="10"/>
-      <c r="P29" s="3"/>
-    </row>
-    <row r="30" spans="2:16" ht="19" customHeight="1">
-      <c r="B30" s="61" t="s">
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="11"/>
+      <c r="P30" s="3"/>
+    </row>
+    <row r="31" spans="2:16" ht="19" customHeight="1">
+      <c r="B31" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="63"/>
-      <c r="D30" s="63"/>
-      <c r="E30" s="63"/>
-      <c r="F30" s="63"/>
-      <c r="G30" s="63"/>
-      <c r="H30" s="64"/>
-      <c r="I30" s="66" t="s">
+      <c r="C31" s="66"/>
+      <c r="D31" s="67"/>
+      <c r="E31" s="67"/>
+      <c r="F31" s="67"/>
+      <c r="G31" s="67"/>
+      <c r="H31" s="68"/>
+      <c r="I31" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="J30" s="67"/>
-      <c r="K30" s="67"/>
-      <c r="L30" s="63"/>
-      <c r="M30" s="63"/>
-      <c r="N30" s="63"/>
-      <c r="O30" s="62"/>
-      <c r="P30" s="1"/>
-    </row>
-    <row r="31" spans="2:16" ht="118.75" customHeight="1">
-      <c r="B31" s="11"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="12"/>
-      <c r="J31" s="12"/>
-      <c r="K31" s="12"/>
-      <c r="L31" s="12"/>
-      <c r="M31" s="12"/>
-      <c r="N31" s="12"/>
-      <c r="O31" s="13"/>
-      <c r="P31" s="2"/>
-    </row>
-    <row r="32" spans="2:16" ht="90" customHeight="1"/>
+      <c r="J31" s="66"/>
+      <c r="K31" s="66"/>
+      <c r="L31" s="67"/>
+      <c r="M31" s="67"/>
+      <c r="N31" s="67"/>
+      <c r="O31" s="64"/>
+      <c r="P31" s="1"/>
+    </row>
+    <row r="32" spans="2:16" ht="118.75" customHeight="1">
+      <c r="B32" s="12"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="14"/>
+      <c r="P32" s="2"/>
+    </row>
+    <row r="33" ht="90" customHeight="1"/>
   </sheetData>
-  <mergeCells count="54">
-    <mergeCell ref="C30:H30"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="H24:K24"/>
-    <mergeCell ref="L24:N24"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="L30:N30"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="L26:N26"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="F26:H26"/>
+  <mergeCells count="58">
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="L27:N27"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:H31"/>
+    <mergeCell ref="I31:K31"/>
+    <mergeCell ref="L31:N31"/>
     <mergeCell ref="B1:P1"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:O3"/>
@@ -1936,7 +1948,10 @@
     <mergeCell ref="J13:O13"/>
     <mergeCell ref="B14:O14"/>
     <mergeCell ref="B15:O15"/>
-    <mergeCell ref="L23:O23"/>
+    <mergeCell ref="L24:O24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="I25:J25"/>
     <mergeCell ref="B18:N18"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="E19:F20"/>
@@ -1944,18 +1959,21 @@
     <mergeCell ref="K19:L19"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="I20:J20"/>
-    <mergeCell ref="B29:O29"/>
-    <mergeCell ref="B31:O31"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="H23:K23"/>
+    <mergeCell ref="L23:O23"/>
+    <mergeCell ref="B30:O30"/>
+    <mergeCell ref="B32:O32"/>
     <mergeCell ref="N19:N20"/>
     <mergeCell ref="B21:O21"/>
-    <mergeCell ref="B25:O25"/>
-    <mergeCell ref="B27:O27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="B26:O26"/>
+    <mergeCell ref="B28:O28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="I29:J29"/>
     <mergeCell ref="B22:O22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="H23:K23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="H24:K24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="69" orientation="portrait" r:id="rId1"/>

</xml_diff>